<commit_message>
Ponpeco Kids' Clothes - 3237739433 업데이트
</commit_message>
<xml_diff>
--- a/Data/Ponpeco Kids' Clothes - 3237739433/3237739433.xlsx
+++ b/Data/Ponpeco Kids' Clothes - 3237739433/3237739433.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Pull Request Here\Ponpeco Kids' Clothes - 3237739433\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\Ponpeco Kids' Clothes - 3237739433\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D6904B-56A9-420B-82DF-4EAF2FB3D0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858D357C-A69C-4863-B5E5-A84CFC09A713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="2840" windowWidth="20080" windowHeight="15850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_240925" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,57 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>bjmi0</author>
+  </authors>
+  <commentList>
+    <comment ref="E49" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-01-12 이전의 원문: '濡れても平気。これにはカエルさんもにっこり'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E57" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-01-12에 새로 추가된 노드들 (12개)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F57" authorId="0" shapeId="0" xr:uid="{42421307-9A36-441E-A799-6E6D71C64189}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-01-12에 새로 추가된 노드들 (12개)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="271">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -63,686 +112,899 @@
     <t>PKC_DecorPlushie.label</t>
   </si>
   <si>
-    <t>A plush toy for decorating a room. It cannot be equipped. Small size.</t>
-  </si>
-  <si>
-    <t>봉제 인형</t>
+    <t>PKC Decorative Plushie S</t>
   </si>
   <si>
     <t>ThingDef+PKC_DecorPlushie.description</t>
   </si>
   <si>
-    <t>PKC_DecorPlushie.description</t>
-  </si>
-  <si>
-    <t>HediffDef+PKCRainCort.label</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKSkirtLeggings.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKSkirtLeggings.label</t>
-  </si>
-  <si>
-    <t>PKC Skirt leggings</t>
-  </si>
-  <si>
-    <t>아동용 레깅스 치마</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKSkirtLeggings.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKSkirtLeggings.description</t>
-  </si>
-  <si>
-    <t>Children's clothing with a layered shirt, skirt, and leggings.</t>
-  </si>
-  <si>
-    <t>셔츠, 치마, 레깅스를 함께 장착하는 아동복입니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKBorderShirt.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKBorderShirt.label</t>
-  </si>
-  <si>
-    <t>PKC Border shirt</t>
-  </si>
-  <si>
-    <t>아동용 줄무늬 셔츠</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKBorderShirt.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKBorderShirt.description</t>
-  </si>
-  <si>
-    <t>A striped shirt for children.</t>
-  </si>
-  <si>
-    <t>아동용 줄무늬 셔츠입니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKCamisoleDress.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKCamisoleDress.label</t>
-  </si>
-  <si>
-    <t>PKC Camisole dress</t>
-  </si>
-  <si>
-    <t>아동용 캐미솔 드레스</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKCamisoleDress.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKCamisoleDress.description</t>
-  </si>
-  <si>
-    <t>A camisole dress for children</t>
-  </si>
-  <si>
-    <t>아동용 캐미솔 드레스입니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKKidsSuit.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKKidsSuit.label</t>
-  </si>
-  <si>
-    <t>PKC Kids Suit</t>
-  </si>
-  <si>
-    <t>아동용 정장</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKKidsSuit.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKKidsSuit.description</t>
-  </si>
-  <si>
-    <t>A suit for children.</t>
-  </si>
-  <si>
-    <t>아동용 정장입니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKKidsHoodie.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKKidsHoodie.label</t>
-  </si>
-  <si>
-    <t>PKC Kids hoodie</t>
-  </si>
-  <si>
-    <t>아동용 후드티</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKKidsHoodie.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKKidsHoodie.description</t>
-  </si>
-  <si>
-    <t>Cold weather clothing for children</t>
-  </si>
-  <si>
-    <t>추운 곳에서 입는 아동용 후드티입니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKFurCoat.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKFurCoat.label</t>
-  </si>
-  <si>
-    <t>PKC Fur coat</t>
-  </si>
-  <si>
-    <t>아동용 털코트</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKFurCoat.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKFurCoat.description</t>
-  </si>
-  <si>
-    <t>A fluffy jacket for children. Prevents cold.</t>
-  </si>
-  <si>
-    <t>어린이용 푹신한 털코트입니다. 추위를 막아줍니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKKnitVest.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKKnitVest.label</t>
-  </si>
-  <si>
-    <t>PKC Knit vest</t>
-  </si>
-  <si>
-    <t>아동용 니트 조끼</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKKnitVest.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKKnitVest.description</t>
-  </si>
-  <si>
-    <t>Children's knit vest</t>
-  </si>
-  <si>
-    <t>아동용 니트 조끼입니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKFormalOnePiece.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKFormalOnePiece.label</t>
-  </si>
-  <si>
-    <t>PKC Formal one piece</t>
-  </si>
-  <si>
-    <t>아동용 정장 원피스</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKFormalOnePiece.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKFormalOnePiece.description</t>
-  </si>
-  <si>
-    <t>A formal dress for children. It's safe if you have one outfit ready.</t>
-  </si>
-  <si>
-    <t>어린이용 정장 드레스입니다. 한 벌만 준비하면 안전합니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKMedievalGirl.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKMedievalGirl.label</t>
-  </si>
-  <si>
-    <t>PKC Medieval girl</t>
-  </si>
-  <si>
-    <t>아동용 중세 의상 (여)</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKMedievalGirl.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKMedievalGirl.description</t>
-  </si>
-  <si>
-    <t>This is a dress worn by common girls in medieval.</t>
-  </si>
-  <si>
-    <t>중세 시대 일반 소녀들이 입었던 옷입니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKMedievalBoy.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKMedievalBoy.label</t>
-  </si>
-  <si>
-    <t>PKC Medieval boy</t>
-  </si>
-  <si>
-    <t>아동용 중세 의상 (남)</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKMedievalBoy.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKMedievalBoy.description</t>
-  </si>
-  <si>
-    <t>This is a dress worn by common boys in medieval.</t>
-  </si>
-  <si>
-    <t>중세 시대 일반 소년들이 입었던 옷입니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKSummerHoodie.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKSummerHoodie.label</t>
-  </si>
-  <si>
-    <t>PKC Summer hoodie</t>
-  </si>
-  <si>
-    <t>아동용 여름 후드티</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKSummerHoodie.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKSummerHoodie.description</t>
-  </si>
-  <si>
-    <t>A thin, airy hoodie for children. Protects your skin from the summer sun.</t>
-  </si>
-  <si>
-    <t>얇고 통풍이 잘되는 어린이용 후드티입니다. 여름 햇볕으로부터 피부를 보호합니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKCatPajama.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKCatPajama.label</t>
-  </si>
-  <si>
-    <t>PKC Cat pajamas</t>
-  </si>
-  <si>
-    <t>아동용 고앙이 잠옷</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKCatPajama.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKCatPajama.description</t>
-  </si>
-  <si>
-    <t>These are children's pajama suits with attached cat tails. Pairing them with a cat ear hood is recommended.</t>
-  </si>
-  <si>
-    <t>고양이 꼬리가 달린 아동용 잠옷입니다. 고양이 후드와 함께 착용하는 것을 추천합니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKDinoPajama.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKDinoPajama.label</t>
-  </si>
-  <si>
-    <t>PKC Dino pajamas</t>
-  </si>
-  <si>
-    <t>아동용 공룡 잠옷</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKDinoPajama.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKDinoPajama.description</t>
-  </si>
-  <si>
-    <t>These are children's pajama suits with attached dinosaur tails. Pairing them with a dinosaur hood is recommended.</t>
-  </si>
-  <si>
-    <t>공룡 꼬리가 달린 아동용 잠옷입니다. 공룡 후드와 함께 착용하는 것을 추천합니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKCatEarHood.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKCatEarHood.label</t>
-  </si>
-  <si>
-    <t>PKC Cat Ear Hood</t>
-  </si>
-  <si>
-    <t>아동용 고양이 후드</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKCatEarHood.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKCatEarHood.description</t>
-  </si>
-  <si>
-    <t>This is a children's hood with attached cat ears. It is recommended to pair it with cat pajamas for a coordinated look.</t>
-  </si>
-  <si>
-    <t>고양이 귀가 달린 아동용 후드입니다. 고양이 잠옷과 함께 착용하는 것을 추천합니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKDinoHood.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKDinoHood.label</t>
-  </si>
-  <si>
-    <t>PKC Dino Hood</t>
-  </si>
-  <si>
-    <t>아동용 공룡 후드</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKDinoHood.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKDinoHood.description</t>
-  </si>
-  <si>
-    <t>This is a children's hood shaped like a dinosaur. It is recommended to pair it with dinosaur pajamas for a coordinated look.</t>
-  </si>
-  <si>
-    <t>공룡 모양의 아동용 후드입니다. 공룡 잠옷과 함께 착용하는 것을 추천합니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKPlushie.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKPlushie.label</t>
-  </si>
-  <si>
-    <t>PKC Plushie</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKPlushie.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKPlushie.description</t>
-  </si>
-  <si>
-    <t>A stuffed toy that resembles an animal. Equipping it gives you a sense of security, and slightly lowers the chance of a mental breakdown.</t>
-  </si>
-  <si>
-    <t>동물을 닮은 봉제 인형입니다. 인형을 착용하면 안정감을 느끼고 정신적으로 약간 편안해집니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKBranch.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKBranch.label</t>
-  </si>
-  <si>
-    <t>PKC Branch</t>
-  </si>
-  <si>
-    <t>장난감 나뭇가지</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKBranch.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKBranch.description</t>
-  </si>
-  <si>
-    <t>It is a wooden stick that fits comfortably in your hand. Holding it will make you feel better, or it will slightly lower the chance of a mental breakdown. It cannot be used for attacks. "An adult told me not to hurt my friends."</t>
-  </si>
-  <si>
-    <t>손에 딱 맞는 나무 막대기입니다. 들고 있으면 안정감을 느끼고 정신적으로 약간 편안해집니다. 공격에는 사용할 수 없습니다. "어른들이 친구를 때리지 말라고 했어요."</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKSFGirl.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKSFGirl.label</t>
-  </si>
-  <si>
-    <t>PKC SF Girl</t>
-  </si>
-  <si>
-    <t>아동용 공상 과학 의상 (여)</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKSFGirl.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKSFGirl.description</t>
-  </si>
-  <si>
-    <t>Children's clothing with a sci-fi design.</t>
-  </si>
-  <si>
-    <t>공상 과학 디자인의 아동복입니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKSFBoy.label</t>
-  </si>
-  <si>
-    <t>Apparel_PPKSFBoy.label</t>
-  </si>
-  <si>
-    <t>PKC SF Boy</t>
-  </si>
-  <si>
-    <t>아동용 공상 과학 의상 (남)</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKSFBoy.description</t>
-  </si>
-  <si>
-    <t>Apparel_PPKSFBoy.description</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCRoyalBoy.label</t>
-  </si>
-  <si>
-    <t>Apparel_PKCRoyalBoy.label</t>
-  </si>
-  <si>
-    <t>PKC Royal Boy</t>
-  </si>
-  <si>
-    <t>아동용 귀족 의상 (남)</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCRoyalBoy.description</t>
-  </si>
-  <si>
-    <t>Apparel_PKCRoyalBoy.description</t>
-  </si>
-  <si>
-    <t>A luxurious and frilly outfit that makes children look like nobility. Although it appears difficult to move in, the children maintain their speed through their indomitable spirit.</t>
-  </si>
-  <si>
-    <t>아이들을 귀족처럼 보이게 하는 고급스럽고 프릴 장식이 달린 의상입니다. 움직이기 힘들어 보이지만 아이들은 불굴의 정신으로 속도를 유지합니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCRoyalGirl.label</t>
-  </si>
-  <si>
-    <t>Apparel_PKCRoyalGirl.label</t>
-  </si>
-  <si>
-    <t>PKC Royal Girl</t>
-  </si>
-  <si>
-    <t>아동용 귀족 의상 (여)</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCRoyalGirl.description</t>
-  </si>
-  <si>
-    <t>Apparel_PKCRoyalGirl.description</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCBackpack.label</t>
-  </si>
-  <si>
-    <t>Apparel_PKCBackpack.label</t>
-  </si>
-  <si>
-    <t>PKC Backpack</t>
-  </si>
-  <si>
-    <t>아동용 배낭</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCBackpack.description</t>
-  </si>
-  <si>
-    <t>Apparel_PKCBackpack.description</t>
-  </si>
-  <si>
-    <t>A small backpack designed for kids, packed to the brim with stones and toys, leaving no space for additional items. Keeping their precious collection nearby excites them and slightly reduces the chance of mental breaks.</t>
-  </si>
-  <si>
-    <t>아이들을 위해 디자인된 작은 배낭은 돌과 장난감으로 가득 채워져 있어 다른 물건을 넣을 공간이 없습니다. 소중한 수집품을 가까이에 두면 아이들의 흥미를 유발하고 정신적 휴식의 기회를 조금이나마 줄일 수 있습니다.</t>
-  </si>
-  <si>
-    <t>PKC Decorative Plushie S</t>
-  </si>
-  <si>
-    <t>HediffDef</t>
-  </si>
-  <si>
-    <t>PKCRainCort.label</t>
-  </si>
-  <si>
-    <t>PKC Rain Cort</t>
-  </si>
-  <si>
-    <t>HediffDef+PKCRainCort.description</t>
-  </si>
-  <si>
-    <t>PKCRainCort.description</t>
-  </si>
-  <si>
-    <t>ThingDef+PKC_DecorPlushieL.label</t>
-  </si>
-  <si>
-    <t>PKC_DecorPlushieL.label</t>
-  </si>
-  <si>
-    <t>PKC Decorative Plushie L</t>
-  </si>
-  <si>
-    <t>ThingDef+PKC_DecorPlushieL.description</t>
-  </si>
-  <si>
-    <t>PKC_DecorPlushieL.description</t>
-  </si>
-  <si>
-    <t>A plush toy for decorating a room. It cannot be equipped. Large size.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCHeroCape.label</t>
-  </si>
-  <si>
-    <t>Apparel_PKCHeroCape.label</t>
-  </si>
-  <si>
-    <t>PKC Hero(?) Cape</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCHeroCape.description</t>
-  </si>
-  <si>
-    <t>Apparel_PKCHeroCape.description</t>
-  </si>
-  <si>
-    <t>A children's outerwear piece. Just throw on some leftover fabric, and you'll feel like a superhero! Its defense and warmth are low, but it can be made easily with minimal materials.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCRaincoat.label</t>
-  </si>
-  <si>
-    <t>Apparel_PKCRaincoat.label</t>
-  </si>
-  <si>
-    <t>PKC Raincoat</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCRaincoat.description</t>
-  </si>
-  <si>
-    <t>Apparel_PKCRaincoat.description</t>
-  </si>
-  <si>
-    <t>A children's raincoat with a frog mark. Perfect for playing energetically even on rainy days.</t>
-  </si>
-  <si>
-    <t>방을 꾸미기 위한 작은 크기의 봉제 인형입니다. 장착할 수 없습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>소형 봉제 인형</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>대형 봉제 인형</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>방을 꾸미기 위한 큰 크기의 봉제 인형입니다. 장착할 수 없습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>濡れても平</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="MS Gothic"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>気</t>
-    </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="맑은 고딕"/>
         <family val="2"/>
-        <charset val="129"/>
       </rPr>
-      <t>。これにはカエルさんもにっこり</t>
+      <t>소형 봉제 인형</t>
     </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>PKC_DecorPlushie.description</t>
+  </si>
+  <si>
+    <t>A plush toy for decorating a room. It cannot be equipped. Small size.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKSkirtLeggings.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>방을 꾸미기 위한 작은 크기의 봉제 인형입니다. 장착할 수 없습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PPKSkirtLeggings.label</t>
+  </si>
+  <si>
+    <t>PKC Skirt leggings</t>
+  </si>
+  <si>
+    <t>아동용 레깅스 치마</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKSkirtLeggings.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKSkirtLeggings.description</t>
+  </si>
+  <si>
+    <t>Children's clothing with a layered shirt, skirt, and leggings.</t>
+  </si>
+  <si>
+    <t>셔츠, 치마, 레깅스를 함께 장착하는 아동복입니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKBorderShirt.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKBorderShirt.label</t>
+  </si>
+  <si>
+    <t>PKC Border shirt</t>
+  </si>
+  <si>
+    <t>아동용 줄무늬 셔츠</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKBorderShirt.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKBorderShirt.description</t>
+  </si>
+  <si>
+    <t>A striped shirt for children.</t>
+  </si>
+  <si>
+    <t>아동용 줄무늬 셔츠입니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKCamisoleDress.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKCamisoleDress.label</t>
+  </si>
+  <si>
+    <t>PKC Camisole dress</t>
+  </si>
+  <si>
+    <t>아동용 캐미솔 드레스</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKCamisoleDress.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKCamisoleDress.description</t>
+  </si>
+  <si>
+    <t>A camisole dress for children</t>
+  </si>
+  <si>
+    <t>아동용 캐미솔 드레스입니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKKidsSuit.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKKidsSuit.label</t>
+  </si>
+  <si>
+    <t>PKC Kids Suit</t>
+  </si>
+  <si>
+    <t>아동용 정장</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKKidsSuit.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKKidsSuit.description</t>
+  </si>
+  <si>
+    <t>A suit for children.</t>
+  </si>
+  <si>
+    <t>아동용 정장입니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKKidsHoodie.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKKidsHoodie.label</t>
+  </si>
+  <si>
+    <t>PKC Kids hoodie</t>
+  </si>
+  <si>
+    <t>아동용 후드티</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKKidsHoodie.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKKidsHoodie.description</t>
+  </si>
+  <si>
+    <t>Cold weather clothing for children</t>
+  </si>
+  <si>
+    <t>추운 곳에서 입는 아동용 후드티입니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKFurCoat.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKFurCoat.label</t>
+  </si>
+  <si>
+    <t>PKC Fur coat</t>
+  </si>
+  <si>
+    <t>아동용 털코트</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKFurCoat.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKFurCoat.description</t>
+  </si>
+  <si>
+    <t>A fluffy jacket for children. Prevents cold.</t>
+  </si>
+  <si>
+    <t>어린이용 푹신한 털코트입니다. 추위를 막아줍니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKKnitVest.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKKnitVest.label</t>
+  </si>
+  <si>
+    <t>PKC Knit vest</t>
+  </si>
+  <si>
+    <t>아동용 니트 조끼</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKKnitVest.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKKnitVest.description</t>
+  </si>
+  <si>
+    <t>Children's knit vest</t>
+  </si>
+  <si>
+    <t>아동용 니트 조끼입니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKFormalOnePiece.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKFormalOnePiece.label</t>
+  </si>
+  <si>
+    <t>PKC Formal one piece</t>
+  </si>
+  <si>
+    <t>아동용 정장 원피스</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKFormalOnePiece.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKFormalOnePiece.description</t>
+  </si>
+  <si>
+    <t>A formal dress for children. It's safe if you have one outfit ready.</t>
+  </si>
+  <si>
+    <t>어린이용 정장 드레스입니다. 한 벌만 준비하면 안전합니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKMedievalGirl.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKMedievalGirl.label</t>
+  </si>
+  <si>
+    <t>PKC Medieval girl</t>
+  </si>
+  <si>
+    <t>아동용 중세 의상 (여)</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKMedievalGirl.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKMedievalGirl.description</t>
+  </si>
+  <si>
+    <t>This is a dress worn by common girls in medieval.</t>
+  </si>
+  <si>
+    <t>중세 시대 일반 소녀들이 입었던 옷입니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKMedievalBoy.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKMedievalBoy.label</t>
+  </si>
+  <si>
+    <t>PKC Medieval boy</t>
+  </si>
+  <si>
+    <t>아동용 중세 의상 (남)</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKMedievalBoy.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKMedievalBoy.description</t>
+  </si>
+  <si>
+    <t>This is a dress worn by common boys in medieval.</t>
+  </si>
+  <si>
+    <t>중세 시대 일반 소년들이 입었던 옷입니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKSummerHoodie.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKSummerHoodie.label</t>
+  </si>
+  <si>
+    <t>PKC Summer hoodie</t>
+  </si>
+  <si>
+    <t>아동용 여름 후드티</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKSummerHoodie.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKSummerHoodie.description</t>
+  </si>
+  <si>
+    <t>A thin, airy hoodie for children. Protects your skin from the summer sun.</t>
+  </si>
+  <si>
+    <t>얇고 통풍이 잘되는 어린이용 후드티입니다. 여름 햇볕으로부터 피부를 보호합니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKCatPajama.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKCatPajama.label</t>
+  </si>
+  <si>
+    <t>PKC Cat pajamas</t>
+  </si>
+  <si>
+    <t>아동용 고앙이 잠옷</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKCatPajama.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKCatPajama.description</t>
+  </si>
+  <si>
+    <t>These are children's pajama suits with attached cat tails. Pairing them with a cat ear hood is recommended.</t>
+  </si>
+  <si>
+    <t>고양이 꼬리가 달린 아동용 잠옷입니다. 고양이 후드와 함께 착용하는 것을 추천합니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKDinoPajama.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKDinoPajama.label</t>
+  </si>
+  <si>
+    <t>PKC Dino pajamas</t>
+  </si>
+  <si>
+    <t>아동용 공룡 잠옷</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKDinoPajama.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKDinoPajama.description</t>
+  </si>
+  <si>
+    <t>These are children's pajama suits with attached dinosaur tails. Pairing them with a dinosaur hood is recommended.</t>
+  </si>
+  <si>
+    <t>공룡 꼬리가 달린 아동용 잠옷입니다. 공룡 후드와 함께 착용하는 것을 추천합니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKCatEarHood.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKCatEarHood.label</t>
+  </si>
+  <si>
+    <t>PKC Cat Ear Hood</t>
+  </si>
+  <si>
+    <t>아동용 고양이 후드</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKCatEarHood.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKCatEarHood.description</t>
+  </si>
+  <si>
+    <t>This is a children's hood with attached cat ears. It is recommended to pair it with cat pajamas for a coordinated look.</t>
+  </si>
+  <si>
+    <t>고양이 귀가 달린 아동용 후드입니다. 고양이 잠옷과 함께 착용하는 것을 추천합니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKDinoHood.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKDinoHood.label</t>
+  </si>
+  <si>
+    <t>PKC Dino Hood</t>
+  </si>
+  <si>
+    <t>아동용 공룡 후드</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKDinoHood.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKDinoHood.description</t>
+  </si>
+  <si>
+    <t>This is a children's hood shaped like a dinosaur. It is recommended to pair it with dinosaur pajamas for a coordinated look.</t>
+  </si>
+  <si>
+    <t>공룡 모양의 아동용 후드입니다. 공룡 잠옷과 함께 착용하는 것을 추천합니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKPlushie.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKPlushie.label</t>
+  </si>
+  <si>
+    <t>PKC Plushie</t>
+  </si>
+  <si>
+    <t>봉제 인형</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKPlushie.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKPlushie.description</t>
+  </si>
+  <si>
+    <t>A stuffed toy that resembles an animal. Equipping it gives you a sense of security, and slightly lowers the chance of a mental breakdown.</t>
+  </si>
+  <si>
+    <t>동물을 닮은 봉제 인형입니다. 인형을 착용하면 안정감을 느끼고 정신적으로 약간 편안해집니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKBranch.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKBranch.label</t>
+  </si>
+  <si>
+    <t>PKC Branch</t>
+  </si>
+  <si>
+    <t>장난감 나뭇가지</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKBranch.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKBranch.description</t>
+  </si>
+  <si>
+    <t>It is a wooden stick that fits comfortably in your hand. Holding it will make you feel better, or it will slightly lower the chance of a mental breakdown. It cannot be used for attacks. "An adult told me not to hurt my friends."</t>
+  </si>
+  <si>
+    <t>손에 딱 맞는 나무 막대기입니다. 들고 있으면 안정감을 느끼고 정신적으로 약간 편안해집니다. 공격에는 사용할 수 없습니다. "어른들이 친구를 때리지 말라고 했어요."</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKSFGirl.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKSFGirl.label</t>
+  </si>
+  <si>
+    <t>PKC SF Girl</t>
+  </si>
+  <si>
+    <t>아동용 공상 과학 의상 (여)</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKSFGirl.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKSFGirl.description</t>
+  </si>
+  <si>
+    <t>Children's clothing with a sci-fi design.</t>
+  </si>
+  <si>
+    <t>공상 과학 디자인의 아동복입니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKSFBoy.label</t>
+  </si>
+  <si>
+    <t>Apparel_PPKSFBoy.label</t>
+  </si>
+  <si>
+    <t>PKC SF Boy</t>
+  </si>
+  <si>
+    <t>아동용 공상 과학 의상 (남)</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PPKSFBoy.description</t>
+  </si>
+  <si>
+    <t>Apparel_PPKSFBoy.description</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCRoyalBoy.label</t>
+  </si>
+  <si>
+    <t>Apparel_PKCRoyalBoy.label</t>
+  </si>
+  <si>
+    <t>PKC Royal Boy</t>
+  </si>
+  <si>
+    <t>아동용 귀족 의상 (남)</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCRoyalBoy.description</t>
+  </si>
+  <si>
+    <t>Apparel_PKCRoyalBoy.description</t>
+  </si>
+  <si>
+    <t>A luxurious and frilly outfit that makes children look like nobility. Although it appears difficult to move in, the children maintain their speed through their indomitable spirit.</t>
+  </si>
+  <si>
+    <t>아이들을 귀족처럼 보이게 하는 고급스럽고 프릴 장식이 달린 의상입니다. 움직이기 힘들어 보이지만 아이들은 불굴의 정신으로 속도를 유지합니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCRoyalGirl.label</t>
+  </si>
+  <si>
+    <t>Apparel_PKCRoyalGirl.label</t>
+  </si>
+  <si>
+    <t>PKC Royal Girl</t>
+  </si>
+  <si>
+    <t>아동용 귀족 의상 (여)</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCRoyalGirl.description</t>
+  </si>
+  <si>
+    <t>Apparel_PKCRoyalGirl.description</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCBackpack.label</t>
+  </si>
+  <si>
+    <t>Apparel_PKCBackpack.label</t>
+  </si>
+  <si>
+    <t>PKC Backpack</t>
+  </si>
+  <si>
+    <t>아동용 배낭</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCBackpack.description</t>
+  </si>
+  <si>
+    <t>Apparel_PKCBackpack.description</t>
+  </si>
+  <si>
+    <t>A small backpack designed for kids, packed to the brim with stones and toys, leaving no space for additional items. Keeping their precious collection nearby excites them and slightly reduces the chance of mental breaks.</t>
+  </si>
+  <si>
+    <t>아이들을 위해 디자인된 작은 배낭은 돌과 장난감으로 가득 채워져 있어 다른 물건을 넣을 공간이 없습니다. 소중한 수집품을 가까이에 두면 아이들의 흥미를 유발하고 정신적 휴식의 기회를 조금이나마 줄일 수 있습니다.</t>
+  </si>
+  <si>
+    <t>HediffDef+PKCRainCort.label</t>
+  </si>
+  <si>
+    <t>HediffDef</t>
+  </si>
+  <si>
+    <t>PKCRainCort.label</t>
+  </si>
+  <si>
+    <t>PKC Rain Cort</t>
+  </si>
+  <si>
+    <t>HediffDef+PKCRainCort.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>개구리 우비</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>PKCRainCort.description</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHalloweenWitch.label</t>
+  </si>
+  <si>
+    <t>ThingDef+PKC_DecorPlushieL.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>비가 오는 날에도 즐겁게 웃을 수 있습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>PKC_DecorPlushieL.label</t>
+  </si>
+  <si>
+    <t>PKC Decorative Plushie L</t>
+  </si>
+  <si>
+    <t>ThingDef+PKC_DecorPlushieL.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>대형 봉제 인형</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>PKC_DecorPlushieL.description</t>
+  </si>
+  <si>
+    <t>A plush toy for decorating a room. It cannot be equipped. Large size.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHeroCape.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>방을 꾸미기 위한 큰 크기의 봉제 인형입니다. 장착할 수 없습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PKCHeroCape.label</t>
+  </si>
+  <si>
+    <t>PKC Hero(?) Cape</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHeroCape.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>아동용 망토</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PKCHeroCape.description</t>
+  </si>
+  <si>
+    <t>A children's outerwear piece. Just throw on some leftover fabric, and you'll feel like a superhero! Its defense and warmth are low, but it can be made easily with minimal materials.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCRaincoat.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>아동용 외투입니다. 천조각을 걸치면 슈퍼 히어로가 된 기분이 듭니다. 방어력과 보온성은 낮지만 최소한의 재료로 쉽게 만들 수 있습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PKCRaincoat.label</t>
+  </si>
+  <si>
+    <t>PKC Raincoat</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCRaincoat.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>아동용 우비</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PKCRaincoat.description</t>
+  </si>
+  <si>
+    <t>A children's raincoat with a frog mark. Perfect for playing energetically even on rainy days.</t>
+  </si>
+  <si>
+    <t>PKC Decorative Plushie</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>개구리 장식이 달린 아동용 우비입니다. 비오는 날에도 활기차게 놀기에 적합합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>A plush toy for decorating a room. It cannot be equipped.</t>
+  </si>
+  <si>
+    <t>방을 꾸미기 위한 봉제 인형입니다. 장착할 수 없습니다.</t>
+  </si>
+  <si>
+    <t>While wearing the raincoat, mood will not decrease even if wet by rain.</t>
+  </si>
+  <si>
+    <t>Apparel_PKCHalloweenWitch.label</t>
+  </si>
+  <si>
+    <t>PKC Halloween Witch</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHalloweenWitch.description</t>
+  </si>
+  <si>
+    <t>Apparel_PKCHalloweenWitch.description</t>
+  </si>
+  <si>
+    <t>Designed for children, this witch-themed costume will make Halloween night magical. Equip the matching pointed hat and enjoy trick-or-treating!</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHalloweenWerewolf.label</t>
+  </si>
+  <si>
+    <t>Apparel_PKCHalloweenWerewolf.label</t>
+  </si>
+  <si>
+    <t>PKC Halloween Werewolf</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHalloweenWerewolf.description</t>
+  </si>
+  <si>
+    <t>Apparel_PKCHalloweenWerewolf.description</t>
+  </si>
+  <si>
+    <t>This children's costume is inspired by werewolves. Equip the werewolf hood too and immerse yourself in the beastly spirit this Halloween! Happy Halloween!</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHWitchHat.label</t>
+  </si>
+  <si>
+    <t>Apparel_PKCHWitchHat.label</t>
+  </si>
+  <si>
+    <t>PKC WitchHat</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHWitchHat.description</t>
+  </si>
+  <si>
+    <t>Apparel_PKCHWitchHat.description</t>
+  </si>
+  <si>
+    <t>The perfect pointed witch hat for Halloween night. An essential item to enhance your costume and make your celebrations more fun.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHWerewolfHood.label</t>
+  </si>
+  <si>
+    <t>Apparel_PKCHWerewolfHood.label</t>
+  </si>
+  <si>
+    <t>PKC Werewolf Hood</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHWerewolfHood.description</t>
+  </si>
+  <si>
+    <t>Apparel_PKCHWerewolfHood.description</t>
+  </si>
+  <si>
+    <t>A hood designed for a full werewolf transformation. It's a bit prickly, but that adds to the authentic werewolf experience.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCCheckedCoat.label</t>
+  </si>
+  <si>
+    <t>Apparel_PKCCheckedCoat.label</t>
+  </si>
+  <si>
+    <t>PKC Checked Coat</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCCheckedCoat.description</t>
+  </si>
+  <si>
+    <t>Apparel_PKCCheckedCoat.description</t>
+  </si>
+  <si>
+    <t>A cozy coat for kids featuring a plaid pattern. The fleece-lined interior keeps them warm even on chilly days! Perfect for outdoor adventures.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCCheckedHood.label</t>
+  </si>
+  <si>
+    <t>Apparel_PKCCheckedHood.label</t>
+  </si>
+  <si>
+    <t>PKC Checked Hood</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCCheckedHood.description</t>
+  </si>
+  <si>
+    <t>Apparel_PKCCheckedHood.description</t>
+  </si>
+  <si>
+    <t>A plaid-patterned hood designed for kids. With its fleece lining, it provides warmth on cold days, making outdoor playtime more enjoyable. Offers the same functionality as a Tuque.</t>
+  </si>
+  <si>
+    <t>할로윈 밤을 마법처럼 만들어줄 마녀 테마의 의상입니다. 마녀 모자와 함께 착용하고 트릭 오어 트릿을 즐기세요!</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>개구리 우비</t>
+    <t>아동용 할로윈 마녀 의상</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>비가 오는 날에도 즐겁게 웃을 수 있습니다.</t>
+    <t>아동용 할로윈 늑대인간 의상</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>아동용 외투입니다. 천조각을 걸치면 슈퍼 히어로가 된 기분이 듭니다. 방어력과 보온성은 낮지만 최소한의 재료로 쉽게 만들 수 있습니다.</t>
+    <t>늑대인간의 모습을 흉내낸 할로윈 코스튬입니다. 늑대인간 모자와 함께 착용하고 할로윈을 즐기세요!</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>아동용 망토</t>
+    <t>아동용 할로윈 마녀 모자</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>아동용 우비</t>
+    <t>할로윈 밤을 마법처럼 만들어줄 마녀 테마의 모자입니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>개구리 장식이 달린 아동용 우비입니다. 비오는 날에도 활기차게 놀기에 적합합니다.</t>
+    <t>아동용 할로윈 늑대인간 모자</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>방을 꾸미기 위한 봉제 인형입니다. 장착할 수 없습니다.</t>
-  </si>
-  <si>
-    <t>A plush toy for decorating a room. It cannot be equipped.</t>
-  </si>
-  <si>
-    <t>PKC Decorative Plushie</t>
+    <t>완전한 늑대인간의 모습을 위해 만들어진 모자입니다. 진정한 늑대인간이 되어 보세요.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>아동용 체크무늬 코트</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>아동용 체크무니 모자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>체크무늬로 장식된 포근한 아동용 코트입니다. 내부가 털실 안감으로 마감되어 쌀쌀한 날에 야외활동을 나가기 좋습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>체크무늬로 장식된 포근한 아동용 모자입니다. 내부가 털실 안감으로 마감되어 쌀쌀한 날에 야외활동을 나가기 좋습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -762,18 +1024,10 @@
       <charset val="129"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="MS Gothic"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <charset val="129"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1112,11 +1366,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="C47" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1162,15 +1416,15 @@
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>185</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>210</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -1179,10 +1433,10 @@
         <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>209</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -1193,885 +1447,1090 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>10</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>13</v>
+        <v>187</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>213</v>
+        <v>193</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A65" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A66" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A67" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A68" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2091,7 +2550,8 @@
     <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.54296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="44.36328125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="9.1796875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -2125,15 +2585,15 @@
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -2145,7 +2605,7 @@
         <v>221</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -2156,744 +2616,744 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>10</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ponpeco Kids' Clothes 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Ponpeco Kids' Clothes - 3237739433/3237739433.xlsx
+++ b/Data/Ponpeco Kids' Clothes - 3237739433/3237739433.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\Ponpeco Kids' Clothes - 3237739433\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858D357C-A69C-4863-B5E5-A84CFC09A713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B9A1DF-D686-4F61-9703-ED97B6F98B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F57" authorId="0" shapeId="0" xr:uid="{42421307-9A36-441E-A799-6E6D71C64189}">
+    <comment ref="F57" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -78,12 +78,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="E69" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-05-02에 새로 추가된 노드들 (10개)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F69" authorId="0" shapeId="0" xr:uid="{9422DA06-1839-486D-94CF-DCF9DD81A9B5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-05-02에 새로 추가된 노드들 (10개)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="311">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -113,9 +139,6 @@
   </si>
   <si>
     <t>PKC Decorative Plushie S</t>
-  </si>
-  <si>
-    <t>ThingDef+PKC_DecorPlushie.description</t>
   </si>
   <si>
     <r>
@@ -130,13 +153,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>ThingDef+PKC_DecorPlushie.description</t>
+  </si>
+  <si>
     <t>PKC_DecorPlushie.description</t>
   </si>
   <si>
     <t>A plush toy for decorating a room. It cannot be equipped. Small size.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PPKSkirtLeggings.label</t>
   </si>
   <si>
     <r>
@@ -151,6 +174,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>ThingDef+Apparel_PPKSkirtLeggings.label</t>
+  </si>
+  <si>
     <t>Apparel_PPKSkirtLeggings.label</t>
   </si>
   <si>
@@ -674,9 +700,6 @@
   </si>
   <si>
     <t>PKC Rain Cort</t>
-  </si>
-  <si>
-    <t>HediffDef+PKCRainCort.description</t>
   </si>
   <si>
     <r>
@@ -691,13 +714,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>HediffDef+PKCRainCort.description</t>
+  </si>
+  <si>
     <t>PKCRainCort.description</t>
   </si>
   <si>
-    <t>ThingDef+Apparel_PKCHalloweenWitch.label</t>
-  </si>
-  <si>
-    <t>ThingDef+PKC_DecorPlushieL.label</t>
+    <t>While wearing the raincoat, mood will not decrease even if wet by rain.</t>
   </si>
   <si>
     <r>
@@ -712,13 +735,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>ThingDef+PKC_DecorPlushieL.label</t>
+  </si>
+  <si>
     <t>PKC_DecorPlushieL.label</t>
   </si>
   <si>
     <t>PKC Decorative Plushie L</t>
-  </si>
-  <si>
-    <t>ThingDef+PKC_DecorPlushieL.description</t>
   </si>
   <si>
     <r>
@@ -733,13 +756,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>ThingDef+PKC_DecorPlushieL.description</t>
+  </si>
+  <si>
     <t>PKC_DecorPlushieL.description</t>
   </si>
   <si>
     <t>A plush toy for decorating a room. It cannot be equipped. Large size.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCHeroCape.label</t>
   </si>
   <si>
     <r>
@@ -754,6 +777,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>ThingDef+Apparel_PKCHeroCape.label</t>
+  </si>
+  <si>
     <t>Apparel_PKCHeroCape.label</t>
   </si>
   <si>
@@ -763,25 +789,10 @@
     <t>ThingDef+Apparel_PKCHeroCape.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>아동용 망토</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PKCHeroCape.description</t>
   </si>
   <si>
     <t>A children's outerwear piece. Just throw on some leftover fabric, and you'll feel like a superhero! Its defense and warmth are low, but it can be made easily with minimal materials.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCRaincoat.label</t>
   </si>
   <si>
     <r>
@@ -796,13 +807,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>ThingDef+Apparel_PKCRaincoat.label</t>
+  </si>
+  <si>
     <t>Apparel_PKCRaincoat.label</t>
   </si>
   <si>
     <t>PKC Raincoat</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCRaincoat.description</t>
   </si>
   <si>
     <r>
@@ -817,13 +828,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>ThingDef+Apparel_PKCRaincoat.description</t>
+  </si>
+  <si>
     <t>Apparel_PKCRaincoat.description</t>
   </si>
   <si>
     <t>A children's raincoat with a frog mark. Perfect for playing energetically even on rainy days.</t>
-  </si>
-  <si>
-    <t>PKC Decorative Plushie</t>
   </si>
   <si>
     <r>
@@ -838,165 +849,396 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>ThingDef+Apparel_PKCHalloweenWitch.label</t>
+  </si>
+  <si>
+    <t>Apparel_PKCHalloweenWitch.label</t>
+  </si>
+  <si>
+    <t>PKC Halloween Witch</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHalloweenWitch.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>아동용 할로윈 마녀 의상</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PKCHalloweenWitch.description</t>
+  </si>
+  <si>
+    <t>Designed for children, this witch-themed costume will make Halloween night magical. Equip the matching pointed hat and enjoy trick-or-treating!</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHalloweenWerewolf.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>할로윈 밤을 마법처럼 만들어줄 마녀 테마의 의상입니다. 마녀 모자와 함께 착용하고 트릭 오어 트릿을 즐기세요!</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PKCHalloweenWerewolf.label</t>
+  </si>
+  <si>
+    <t>PKC Halloween Werewolf</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHalloweenWerewolf.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>아동용 할로윈 늑대인간 의상</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PKCHalloweenWerewolf.description</t>
+  </si>
+  <si>
+    <t>This children's costume is inspired by werewolves. Equip the werewolf hood too and immerse yourself in the beastly spirit this Halloween! Happy Halloween!</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHWitchHat.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>늑대인간의 모습을 흉내낸 할로윈 코스튬입니다. 늑대인간 모자와 함께 착용하고 할로윈을 즐기세요!</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PKCHWitchHat.label</t>
+  </si>
+  <si>
+    <t>PKC WitchHat</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHWitchHat.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>아동용 할로윈 마녀 모자</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PKCHWitchHat.description</t>
+  </si>
+  <si>
+    <t>The perfect pointed witch hat for Halloween night. An essential item to enhance your costume and make your celebrations more fun.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHWerewolfHood.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>할로윈 밤을 마법처럼 만들어줄 마녀 테마의 모자입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PKCHWerewolfHood.label</t>
+  </si>
+  <si>
+    <t>PKC Werewolf Hood</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHWerewolfHood.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>아동용 할로윈 늑대인간 모자</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PKCHWerewolfHood.description</t>
+  </si>
+  <si>
+    <t>A hood designed for a full werewolf transformation. It's a bit prickly, but that adds to the authentic werewolf experience.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCCheckedCoat.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>완전한 늑대인간의 모습을 위해 만들어진 모자입니다. 진정한 늑대인간이 되어 보세요.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PKCCheckedCoat.label</t>
+  </si>
+  <si>
+    <t>PKC Checked Coat</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCCheckedCoat.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>아동용 체크무늬 코트</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PKCCheckedCoat.description</t>
+  </si>
+  <si>
+    <t>A cozy coat for kids featuring a plaid pattern. The fleece-lined interior keeps them warm even on chilly days! Perfect for outdoor adventures.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCCheckedHood.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>체크무늬로 장식된 포근한 아동용 코트입니다. 내부가 털실 안감으로 마감되어 쌀쌀한 날에 야외활동을 나가기 좋습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PKCCheckedHood.label</t>
+  </si>
+  <si>
+    <t>PKC Checked Hood</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCCheckedHood.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>아동용 체크무니 모자</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PKCCheckedHood.description</t>
+  </si>
+  <si>
+    <t>A plaid-patterned hood designed for kids. With its fleece lining, it provides warmth on cold days, making outdoor playtime more enjoyable. Offers the same functionality as a Tuque.</t>
+  </si>
+  <si>
+    <t>PKC Decorative Plushie</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>체크무늬로 장식된 포근한 아동용 모자입니다. 내부가 털실 안감으로 마감되어 쌀쌀한 날에 야외활동을 나가기 좋습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>A plush toy for decorating a room. It cannot be equipped.</t>
   </si>
   <si>
     <t>방을 꾸미기 위한 봉제 인형입니다. 장착할 수 없습니다.</t>
   </si>
   <si>
-    <t>While wearing the raincoat, mood will not decrease even if wet by rain.</t>
-  </si>
-  <si>
-    <t>Apparel_PKCHalloweenWitch.label</t>
-  </si>
-  <si>
-    <t>PKC Halloween Witch</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCHalloweenWitch.description</t>
-  </si>
-  <si>
-    <t>Apparel_PKCHalloweenWitch.description</t>
-  </si>
-  <si>
-    <t>Designed for children, this witch-themed costume will make Halloween night magical. Equip the matching pointed hat and enjoy trick-or-treating!</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCHalloweenWerewolf.label</t>
-  </si>
-  <si>
-    <t>Apparel_PKCHalloweenWerewolf.label</t>
-  </si>
-  <si>
-    <t>PKC Halloween Werewolf</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCHalloweenWerewolf.description</t>
-  </si>
-  <si>
-    <t>Apparel_PKCHalloweenWerewolf.description</t>
-  </si>
-  <si>
-    <t>This children's costume is inspired by werewolves. Equip the werewolf hood too and immerse yourself in the beastly spirit this Halloween! Happy Halloween!</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCHWitchHat.label</t>
-  </si>
-  <si>
-    <t>Apparel_PKCHWitchHat.label</t>
-  </si>
-  <si>
-    <t>PKC WitchHat</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCHWitchHat.description</t>
-  </si>
-  <si>
-    <t>Apparel_PKCHWitchHat.description</t>
-  </si>
-  <si>
-    <t>The perfect pointed witch hat for Halloween night. An essential item to enhance your costume and make your celebrations more fun.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCHWerewolfHood.label</t>
-  </si>
-  <si>
-    <t>Apparel_PKCHWerewolfHood.label</t>
-  </si>
-  <si>
-    <t>PKC Werewolf Hood</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCHWerewolfHood.description</t>
-  </si>
-  <si>
-    <t>Apparel_PKCHWerewolfHood.description</t>
-  </si>
-  <si>
-    <t>A hood designed for a full werewolf transformation. It's a bit prickly, but that adds to the authentic werewolf experience.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCCheckedCoat.label</t>
-  </si>
-  <si>
-    <t>Apparel_PKCCheckedCoat.label</t>
-  </si>
-  <si>
-    <t>PKC Checked Coat</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCCheckedCoat.description</t>
-  </si>
-  <si>
-    <t>Apparel_PKCCheckedCoat.description</t>
-  </si>
-  <si>
-    <t>A cozy coat for kids featuring a plaid pattern. The fleece-lined interior keeps them warm even on chilly days! Perfect for outdoor adventures.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCCheckedHood.label</t>
-  </si>
-  <si>
-    <t>Apparel_PKCCheckedHood.label</t>
-  </si>
-  <si>
-    <t>PKC Checked Hood</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PKCCheckedHood.description</t>
-  </si>
-  <si>
-    <t>Apparel_PKCCheckedHood.description</t>
-  </si>
-  <si>
-    <t>A plaid-patterned hood designed for kids. With its fleece lining, it provides warmth on cold days, making outdoor playtime more enjoyable. Offers the same functionality as a Tuque.</t>
-  </si>
-  <si>
-    <t>할로윈 밤을 마법처럼 만들어줄 마녀 테마의 의상입니다. 마녀 모자와 함께 착용하고 트릭 오어 트릿을 즐기세요!</t>
+    <t>ThingDef+Apparel_PKCHeroHelmet.label</t>
+  </si>
+  <si>
+    <t>Apparel_PKCHeroHelmet.label</t>
+  </si>
+  <si>
+    <t>PKC Hero(?)Helmet</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCHeroHelmet.description</t>
+  </si>
+  <si>
+    <t>Apparel_PKCHeroHelmet.description</t>
+  </si>
+  <si>
+    <t>The legendary hero has finally appeared!\nFeeling like having some stew? Sorry, but that’s no longer an option. This pot has been reborn as the legendary hero’s helmet.\nProvides the same protection as a kid helmet.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCSummerDress.label</t>
+  </si>
+  <si>
+    <t>Apparel_PKCSummerDress.label</t>
+  </si>
+  <si>
+    <t>PKC Summer Dress</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCSummerDress.description</t>
+  </si>
+  <si>
+    <t>Apparel_PKCSummerDress.description</t>
+  </si>
+  <si>
+    <t>A refreshing one-piece dress that catches the eye with its elegant floral pattern.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCSailorSuit.label</t>
+  </si>
+  <si>
+    <t>Apparel_PKCSailorSuit.label</t>
+  </si>
+  <si>
+    <t>PKC Sailor Suit</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCSailorSuit.description</t>
+  </si>
+  <si>
+    <t>Apparel_PKCSailorSuit.description</t>
+  </si>
+  <si>
+    <t>A boys' sailor outfit perfect for summer, with a breezy oversized collar and clean-cut short pants.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCScallopCardigan.label</t>
+  </si>
+  <si>
+    <t>Apparel_PKCScallopCardigan.label</t>
+  </si>
+  <si>
+    <t>PKC Scallop Cardigan</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCScallopCardigan.description</t>
+  </si>
+  <si>
+    <t>Apparel_PKCScallopCardigan.description</t>
+  </si>
+  <si>
+    <t>A special spring-summer cardigan with petal-like scalloped edges on the collar and hem.\nIts airy fabric gently shields you from the sun and offers heat resistance for warm days.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCSailorShirt.label</t>
+  </si>
+  <si>
+    <t>Apparel_PKCSailorShirt.label</t>
+  </si>
+  <si>
+    <t>PKC Sailor Shirt</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PKCSailorShirt.description</t>
+  </si>
+  <si>
+    <t>Apparel_PKCSailorShirt.description</t>
+  </si>
+  <si>
+    <t>A lightweight hoodie with a standout sailor collar and excellent breathability.\nProvides heat resistance to keep you comfortable even in harsh summer sunlight.</t>
+  </si>
+  <si>
+    <t>우아한 꽃무늬가 눈길을 사로잡는 산뜻한 원피스 드레스입니다.</t>
+  </si>
+  <si>
+    <t>시원하게 큰 칼라와 깔끔한 반바지가 특징인, 여름에 완벽한 소년용 세일러복입니다.</t>
+  </si>
+  <si>
+    <t>전설적인 영웅이 마침내 나타났습니다!\n스튜라도 끓여 먹고 싶다고요? 미안하지만, 그럴 수 없게 됐습니다. 이 냄비는 전설적인 영웅의 헬멧으로 다시 태어났거든요.\n아동용 방탄모와 동일한 보호 성능을 제공합니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>아동용 할로윈 마녀 의상</t>
+    <t>아동용 히어로 망토</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>아동용 히어로 모자</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>아동용 할로윈 늑대인간 의상</t>
+    <t>아동용 세일러복</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>늑대인간의 모습을 흉내낸 할로윈 코스튬입니다. 늑대인간 모자와 함께 착용하고 할로윈을 즐기세요!</t>
+    <t>아동용 세일러 셔츠</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>아동용 할로윈 마녀 모자</t>
+    <t>눈에 띄는 세일러 칼라와 뛰어난 통기성을 갖춘 가벼운 후드 셔츠입니다.\n혹독한 여름 햇볕 속에서도 편안함을 유지할 수 있도록 더위 저항을 제공합니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>할로윈 밤을 마법처럼 만들어줄 마녀 테마의 모자입니다.</t>
+    <t>칼라와 밑단에 꽃잎 같은 물결 모양 장식이 있는 특별한 봄-여름 가디건입니다.\n통기성 좋은 원단이 햇볕을 부드럽게 막아주고 더운 날에도 더위 저항을 제공합니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>아동용 할로윈 늑대인간 모자</t>
+    <t>아동용 물결무늬 가디건</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>완전한 늑대인간의 모습을 위해 만들어진 모자입니다. 진정한 늑대인간이 되어 보세요.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>아동용 체크무늬 코트</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>아동용 체크무니 모자</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>체크무늬로 장식된 포근한 아동용 코트입니다. 내부가 털실 안감으로 마감되어 쌀쌀한 날에 야외활동을 나가기 좋습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>체크무늬로 장식된 포근한 아동용 모자입니다. 내부가 털실 안감으로 마감되어 쌀쌀한 날에 야외활동을 나가기 좋습니다.</t>
+    <t>아동용 꽃무늬 드레스</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1367,10 +1609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C47" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1419,12 +1661,12 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -1436,12 +1678,12 @@
         <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -2201,12 +2443,12 @@
         <v>190</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>188</v>
@@ -2215,15 +2457,15 @@
         <v>193</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>7</v>
@@ -2235,12 +2477,12 @@
         <v>198</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>7</v>
@@ -2252,12 +2494,12 @@
         <v>202</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>7</v>
@@ -2269,7 +2511,7 @@
         <v>206</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>208</v>
+        <v>303</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
@@ -2280,13 +2522,13 @@
         <v>7</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
@@ -2297,13 +2539,13 @@
         <v>7</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
@@ -2314,86 +2556,86 @@
         <v>7</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>194</v>
+        <v>219</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>260</v>
+        <v>223</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E59" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>234</v>
-      </c>
       <c r="F60" s="1" t="s">
-        <v>262</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>7</v>
@@ -2405,7 +2647,7 @@
         <v>237</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
@@ -2416,115 +2658,285 @@
         <v>7</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="F68" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A69" s="1" t="s">
         <v>270</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A70" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A71" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A72" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A73" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A74" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A75" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A76" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A77" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A78" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -2585,7 +2997,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>219</v>
+        <v>266</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>138</v>
@@ -2593,7 +3005,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -2602,15 +3014,15 @@
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>221</v>
+        <v>268</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>222</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>

</xml_diff>